<commit_message>
Commited By Sumit Including all the Mobile Part
</commit_message>
<xml_diff>
--- a/Framework/Database/TestDataDB.xlsx
+++ b/Framework/Database/TestDataDB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KalivaradhanS\Desktop\Work_New\VFQA-Parallel\Framework\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Olympus\VFQA-Parallel\Framework\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="316">
   <si>
     <t>Application_Details</t>
   </si>
@@ -613,9 +613,6 @@
     <t>ParallelRun</t>
   </si>
   <si>
-    <t>https://10.162.53.100:4443/ecommunications_oui_enu/start.swe?</t>
-  </si>
-  <si>
     <t>Dependency</t>
   </si>
   <si>
@@ -871,64 +868,121 @@
     <t>Brmsitenv@123</t>
   </si>
   <si>
-    <t>KALISARAVANAN</t>
-  </si>
-  <si>
-    <t>Maveric@2018</t>
+    <t>10.162.53.94</t>
+  </si>
+  <si>
+    <t>HALEEMI</t>
+  </si>
+  <si>
+    <t>XML Invoicegeneration</t>
+  </si>
+  <si>
+    <t>BillSummary</t>
+  </si>
+  <si>
+    <t>DueAmount</t>
+  </si>
+  <si>
+    <t>HappyOffers</t>
+  </si>
+  <si>
+    <t>PJM_Login</t>
+  </si>
+  <si>
+    <t>PJM_Upload</t>
+  </si>
+  <si>
+    <t>PJM_APP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Launching the browser </t>
+  </si>
+  <si>
+    <t>Uploading File</t>
+  </si>
+  <si>
+    <t>ProductDeActivation_USSD_Prepaid</t>
+  </si>
+  <si>
+    <t>VerifyProductDeActivationPrepaid</t>
+  </si>
+  <si>
+    <t>BillEnquiryDialler</t>
+  </si>
+  <si>
+    <t>Extracting Bill via USSD</t>
+  </si>
+  <si>
+    <t>BillPayment_USSD</t>
+  </si>
+  <si>
+    <t>setMCareCapabilities</t>
+  </si>
+  <si>
+    <t>verifyMCareLogin</t>
+  </si>
+  <si>
+    <t>verifyPlanNameMCare</t>
+  </si>
+  <si>
+    <t>billEnquiryMCare</t>
+  </si>
+  <si>
+    <t>Verifying Happy Offers</t>
+  </si>
+  <si>
+    <t>Validating the Bill Amount</t>
+  </si>
+  <si>
+    <t>Capturing the Existing Bill Amount</t>
+  </si>
+  <si>
+    <t>Prepaid_Happy_Offers_USSD</t>
+  </si>
+  <si>
+    <t>Fetching Bill Amount from Siebel</t>
+  </si>
+  <si>
+    <t>BillEnquiry_USSD</t>
+  </si>
+  <si>
+    <t>QA05</t>
   </si>
   <si>
     <t>Batch1</t>
   </si>
   <si>
-    <t>10.162.53.94</t>
-  </si>
-  <si>
-    <t>HALEEMI</t>
-  </si>
-  <si>
-    <t>MultipleAccount</t>
-  </si>
-  <si>
-    <t>XML Invoicegeneration</t>
-  </si>
-  <si>
-    <t>AccountNo--11004935055||Beyond_PVT_Date--03-05-2017 00:00:00M||</t>
-  </si>
-  <si>
-    <t>MultipleAccountNo--11004935055||PVT_Date--050100002018||</t>
-  </si>
-  <si>
-    <t>Prepaid_Happy_Offers</t>
-  </si>
-  <si>
-    <t>Postpaid_Bill_Payment</t>
-  </si>
-  <si>
-    <t>Bill_Enquiry</t>
-  </si>
-  <si>
-    <t>BillSummary</t>
-  </si>
-  <si>
-    <t>DueAmount</t>
-  </si>
-  <si>
-    <t>HappyOffers</t>
-  </si>
-  <si>
-    <t>PJM_Login</t>
-  </si>
-  <si>
-    <t>PJM_Upload</t>
-  </si>
-  <si>
-    <t>PJM_APP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Launching the browser </t>
-  </si>
-  <si>
-    <t>Uploading File</t>
+    <t>MCare_BillEnquiry</t>
+  </si>
+  <si>
+    <t>MCare_VerifyPlanName</t>
+  </si>
+  <si>
+    <t>MVCareBill</t>
+  </si>
+  <si>
+    <t>To Fetch Mcare Fetch</t>
+  </si>
+  <si>
+    <t>MSISDN--97470899060||DeviceName--DeviceOne||Env--Test||</t>
+  </si>
+  <si>
+    <t>MSISDN--97431356005||DeviceName--DeviceOne||USSDMenu--*123#||USSDJourney--#,#,7||</t>
+  </si>
+  <si>
+    <t>https://10.160.222.21:4443/ecommunications_oui_enu/start.swe?</t>
+  </si>
+  <si>
+    <t>HaleemBaig</t>
+  </si>
+  <si>
+    <t>Mav@2018</t>
+  </si>
+  <si>
+    <t>MSISDN--97431356005||DeviceName--DeviceOne||USSDMenu--*100#||USSDJourney--1,3,1||</t>
+  </si>
+  <si>
+    <t>MSISDN--97430992830||DeviceName--DeviceOne||BillEnquiryCode--*122#||</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1086,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1079,22 +1133,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1118,20 +1161,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1607,7 +1648,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,7 +1656,7 @@
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="149.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1645,16 +1686,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>303</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>311</v>
       </c>
       <c r="D2" t="s">
-        <v>278</v>
+        <v>312</v>
       </c>
       <c r="E2" t="s">
-        <v>279</v>
+        <v>313</v>
       </c>
       <c r="F2" t="s">
         <v>125</v>
@@ -1690,30 +1731,30 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" t="s">
         <v>275</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>276</v>
-      </c>
-      <c r="E5" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D6" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E6" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1733,7 +1774,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1742,10 +1783,9 @@
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="86.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1760,7 +1800,7 @@
         <v>191</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>48</v>
@@ -1783,22 +1823,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="D2" t="s">
         <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>306</v>
       </c>
       <c r="F2" t="s">
-        <v>283</v>
+        <v>306</v>
       </c>
       <c r="H2" t="s">
-        <v>286</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1806,22 +1846,68 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="D3" t="s">
         <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>300</v>
       </c>
       <c r="F3" t="s">
-        <v>152</v>
+        <v>300</v>
       </c>
       <c r="H3" t="s">
-        <v>285</v>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F4" t="s">
+        <v>288</v>
+      </c>
+      <c r="H4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H5" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1835,18 +1921,19 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E442"/>
+  <dimension ref="A1:E479"/>
   <sheetViews>
-    <sheetView topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="E261" sqref="E261"/>
+    <sheetView topLeftCell="A446" workbookViewId="0">
+      <selection activeCell="C454" sqref="C454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="32.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2905,7 +2992,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="11"/>
+      <c r="A67" s="15"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
@@ -3129,7 +3216,7 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="11"/>
+      <c r="A81" s="15"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
@@ -3357,7 +3444,7 @@
         <v>1</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>12</v>
@@ -3374,7 +3461,7 @@
         <v>2</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>73</v>
@@ -3391,10 +3478,10 @@
         <v>3</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>15</v>
@@ -3408,7 +3495,7 @@
         <v>4</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>73</v>
@@ -3425,7 +3512,7 @@
         <v>5</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>27</v>
@@ -3442,7 +3529,7 @@
         <v>6</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>29</v>
@@ -3459,7 +3546,7 @@
         <v>7</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>31</v>
@@ -3476,7 +3563,7 @@
         <v>8</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>25</v>
@@ -4193,13 +4280,13 @@
         <v>65</v>
       </c>
       <c r="C153" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D153" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E153" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="D153" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E153" s="6" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4261,13 +4348,13 @@
         <v>66</v>
       </c>
       <c r="C158" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E158" s="6" t="s">
         <v>252</v>
-      </c>
-      <c r="D158" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E158" s="6" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4343,7 +4430,7 @@
         <v>1</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C165" s="5" t="s">
         <v>12</v>
@@ -4360,10 +4447,10 @@
         <v>2</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D166" s="6" t="s">
         <v>15</v>
@@ -4377,7 +4464,7 @@
         <v>3</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C167" s="6" t="s">
         <v>25</v>
@@ -4599,7 +4686,7 @@
         <v>1</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>12</v>
@@ -4616,10 +4703,10 @@
         <v>2</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D186" s="6" t="s">
         <v>15</v>
@@ -4633,7 +4720,7 @@
         <v>3</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C187" s="6" t="s">
         <v>25</v>
@@ -4651,7 +4738,7 @@
         <v>1</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C189" s="6" t="s">
         <v>12</v>
@@ -4668,10 +4755,10 @@
         <v>2</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C190" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D190" s="6" t="s">
         <v>15</v>
@@ -4685,7 +4772,7 @@
         <v>3</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C191" s="6" t="s">
         <v>25</v>
@@ -4703,7 +4790,7 @@
         <v>1</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C193" s="6" t="s">
         <v>12</v>
@@ -4720,10 +4807,10 @@
         <v>2</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C194" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D194" s="6" t="s">
         <v>15</v>
@@ -4737,7 +4824,7 @@
         <v>3</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C195" s="6" t="s">
         <v>25</v>
@@ -4755,7 +4842,7 @@
         <v>1</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C197" s="6" t="s">
         <v>12</v>
@@ -4772,10 +4859,10 @@
         <v>2</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C198" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D198" s="6" t="s">
         <v>15</v>
@@ -4789,7 +4876,7 @@
         <v>3</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C199" s="6" t="s">
         <v>25</v>
@@ -4806,7 +4893,7 @@
         <v>1</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C201" s="6" t="s">
         <v>12</v>
@@ -4823,16 +4910,16 @@
         <v>2</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C202" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D202" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E202" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -4840,7 +4927,7 @@
         <v>3</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>25</v>
@@ -4857,7 +4944,7 @@
         <v>1</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C205" s="6" t="s">
         <v>12</v>
@@ -4874,16 +4961,16 @@
         <v>2</v>
       </c>
       <c r="B206" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C206" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D206" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E206" s="6" t="s">
         <v>264</v>
-      </c>
-      <c r="C206" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="D206" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E206" s="6" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -4891,7 +4978,7 @@
         <v>3</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C207" s="6" t="s">
         <v>25</v>
@@ -4904,18 +4991,18 @@
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A208" s="12"/>
-      <c r="B208" s="12"/>
-      <c r="C208" s="12"/>
-      <c r="D208" s="12"/>
-      <c r="E208" s="12"/>
+      <c r="A208" s="16"/>
+      <c r="B208" s="16"/>
+      <c r="C208" s="16"/>
+      <c r="D208" s="16"/>
+      <c r="E208" s="16"/>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>1</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C209" s="6" t="s">
         <v>12</v>
@@ -4932,16 +5019,16 @@
         <v>2</v>
       </c>
       <c r="B210" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C210" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="D210" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E210" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="C210" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D210" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E210" s="6" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -4949,7 +5036,7 @@
         <v>3</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C211" s="6" t="s">
         <v>25</v>
@@ -4962,11 +5049,11 @@
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A212" s="12"/>
-      <c r="B212" s="12"/>
-      <c r="C212" s="12"/>
-      <c r="D212" s="12"/>
-      <c r="E212" s="12"/>
+      <c r="A212" s="16"/>
+      <c r="B212" s="16"/>
+      <c r="C212" s="16"/>
+      <c r="D212" s="16"/>
+      <c r="E212" s="16"/>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
@@ -5194,7 +5281,7 @@
         <v>1</v>
       </c>
       <c r="B229" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C229" s="6" t="s">
         <v>12</v>
@@ -5211,16 +5298,16 @@
         <v>2</v>
       </c>
       <c r="B230" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C230" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D230" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E230" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="C230" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="D230" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E230" s="6" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -5228,7 +5315,7 @@
         <v>3</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C231" s="6" t="s">
         <v>25</v>
@@ -5245,7 +5332,7 @@
         <v>1</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C233" s="5" t="s">
         <v>12</v>
@@ -5262,10 +5349,10 @@
         <v>2</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D234" s="6" t="s">
         <v>15</v>
@@ -5279,7 +5366,7 @@
         <v>3</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C235" s="5" t="s">
         <v>73</v>
@@ -5296,7 +5383,7 @@
         <v>4</v>
       </c>
       <c r="B236" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C236" s="5" t="s">
         <v>27</v>
@@ -5313,7 +5400,7 @@
         <v>5</v>
       </c>
       <c r="B237" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C237" s="5" t="s">
         <v>29</v>
@@ -5330,7 +5417,7 @@
         <v>6</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C238" s="5" t="s">
         <v>31</v>
@@ -5347,7 +5434,7 @@
         <v>7</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C239" s="5" t="s">
         <v>25</v>
@@ -5487,13 +5574,13 @@
         <v>91</v>
       </c>
       <c r="C250" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D250" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="D250" s="6" t="s">
+      <c r="E250" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="E250" s="6" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -5521,13 +5608,13 @@
         <v>91</v>
       </c>
       <c r="C252" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D252" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E252" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="D252" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E252" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -5572,13 +5659,13 @@
         <v>142</v>
       </c>
       <c r="C256" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D256" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="D256" s="6" t="s">
+      <c r="E256" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="E256" s="6" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -5595,7 +5682,7 @@
         <v>15</v>
       </c>
       <c r="E257" s="6" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -5606,13 +5693,13 @@
         <v>142</v>
       </c>
       <c r="C258" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D258" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E258" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="D258" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E258" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -5640,13 +5727,13 @@
         <v>142</v>
       </c>
       <c r="C260" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="D260" s="6" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="E260" s="6" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -5657,13 +5744,13 @@
         <v>142</v>
       </c>
       <c r="C261" s="6" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D261" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E261" s="6" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -5671,7 +5758,7 @@
         <v>1</v>
       </c>
       <c r="B263" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C263" s="5" t="s">
         <v>12</v>
@@ -5688,16 +5775,16 @@
         <v>2</v>
       </c>
       <c r="B264" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C264" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D264" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E264" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="C264" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D264" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E264" s="6" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -5705,7 +5792,7 @@
         <v>3</v>
       </c>
       <c r="B265" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C265" s="5" t="s">
         <v>25</v>
@@ -5722,16 +5809,16 @@
         <v>4</v>
       </c>
       <c r="B266" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C266" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D266" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="D266" s="6" t="s">
+      <c r="E266" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="E266" s="6" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -5739,16 +5826,16 @@
         <v>5</v>
       </c>
       <c r="B267" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C267" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D267" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E267" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="D267" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E267" s="6" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
@@ -5756,16 +5843,16 @@
         <v>6</v>
       </c>
       <c r="B268" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C268" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D268" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E268" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="D268" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E268" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -5773,7 +5860,7 @@
         <v>7</v>
       </c>
       <c r="B269" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C269" s="5" t="s">
         <v>88</v>
@@ -5790,16 +5877,16 @@
         <v>8</v>
       </c>
       <c r="B270" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C270" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D270" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E270" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="D270" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E270" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="271" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5807,7 +5894,7 @@
         <v>9</v>
       </c>
       <c r="B271" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C271" s="5" t="s">
         <v>86</v>
@@ -5824,7 +5911,7 @@
         <v>1</v>
       </c>
       <c r="B273" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C273" s="5" t="s">
         <v>12</v>
@@ -5841,16 +5928,16 @@
         <v>2</v>
       </c>
       <c r="B274" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C274" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D274" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E274" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="275" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5858,7 +5945,7 @@
         <v>3</v>
       </c>
       <c r="B275" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C275" s="5" t="s">
         <v>25</v>
@@ -5875,7 +5962,7 @@
         <v>1</v>
       </c>
       <c r="B277" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C277" s="5" t="s">
         <v>12</v>
@@ -5892,16 +5979,16 @@
         <v>2</v>
       </c>
       <c r="B278" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C278" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D278" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E278" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="279" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5909,7 +5996,7 @@
         <v>3</v>
       </c>
       <c r="B279" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C279" s="5" t="s">
         <v>25</v>
@@ -5946,13 +6033,13 @@
         <v>138</v>
       </c>
       <c r="C282" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D282" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E282" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="283" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5963,13 +6050,13 @@
         <v>138</v>
       </c>
       <c r="C283" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D283" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E283" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="284" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6018,7 +6105,7 @@
         <v>1</v>
       </c>
       <c r="B287" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C287" s="5" t="s">
         <v>139</v>
@@ -6035,16 +6122,16 @@
         <v>2</v>
       </c>
       <c r="B288" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C288" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D288" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E288" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="289" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6052,16 +6139,16 @@
         <v>3</v>
       </c>
       <c r="B289" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C289" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D289" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E289" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="290" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6069,7 +6156,7 @@
         <v>4</v>
       </c>
       <c r="B290" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C290" s="5" t="s">
         <v>140</v>
@@ -6086,16 +6173,16 @@
         <v>5</v>
       </c>
       <c r="B291" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C291" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C291" s="5" t="s">
+      <c r="D291" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E291" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="D291" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E291" s="6" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -6110,7 +6197,7 @@
         <v>1</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C293" s="5" t="s">
         <v>139</v>
@@ -6127,16 +6214,16 @@
         <v>2</v>
       </c>
       <c r="B294" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C294" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C294" s="5" t="s">
-        <v>221</v>
-      </c>
       <c r="D294" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E294" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="295" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6144,16 +6231,16 @@
         <v>3</v>
       </c>
       <c r="B295" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C295" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D295" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E295" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D295" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E295" s="6" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="296" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6161,7 +6248,7 @@
         <v>4</v>
       </c>
       <c r="B296" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C296" s="5" t="s">
         <v>140</v>
@@ -6178,16 +6265,16 @@
         <v>5</v>
       </c>
       <c r="B297" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C297" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D297" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E297" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
@@ -6202,7 +6289,7 @@
         <v>1</v>
       </c>
       <c r="B299" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C299" s="5" t="s">
         <v>139</v>
@@ -6219,16 +6306,16 @@
         <v>2</v>
       </c>
       <c r="B300" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C300" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D300" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E300" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="301" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6236,16 +6323,16 @@
         <v>3</v>
       </c>
       <c r="B301" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C301" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D301" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E301" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="302" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6253,7 +6340,7 @@
         <v>4</v>
       </c>
       <c r="B302" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C302" s="5" t="s">
         <v>140</v>
@@ -6270,16 +6357,16 @@
         <v>5</v>
       </c>
       <c r="B303" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C303" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="C303" s="5" t="s">
+      <c r="D303" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E303" s="6" t="s">
         <v>226</v>
-      </c>
-      <c r="D303" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E303" s="6" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="305" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6287,16 +6374,16 @@
         <v>1</v>
       </c>
       <c r="B305" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C305" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D305" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E305" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="306" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6304,16 +6391,16 @@
         <v>2</v>
       </c>
       <c r="B306" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C306" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C306" s="5" t="s">
-        <v>229</v>
-      </c>
       <c r="D306" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E306" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="307" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6321,16 +6408,16 @@
         <v>3</v>
       </c>
       <c r="B307" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C307" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D307" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E307" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="308" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6338,16 +6425,16 @@
         <v>4</v>
       </c>
       <c r="B308" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C308" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D308" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E308" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="310" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6355,16 +6442,16 @@
         <v>1</v>
       </c>
       <c r="B310" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C310" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D310" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E310" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="311" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6372,16 +6459,16 @@
         <v>2</v>
       </c>
       <c r="B311" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C311" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D311" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E311" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="312" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6389,16 +6476,16 @@
         <v>3</v>
       </c>
       <c r="B312" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C312" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D312" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E312" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="313" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6406,16 +6493,16 @@
         <v>4</v>
       </c>
       <c r="B313" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C313" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D313" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E313" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="315" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6423,7 +6510,7 @@
         <v>1</v>
       </c>
       <c r="B315" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C315" s="5" t="s">
         <v>139</v>
@@ -6440,16 +6527,16 @@
         <v>2</v>
       </c>
       <c r="B316" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C316" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D316" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E316" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="317" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6457,16 +6544,16 @@
         <v>3</v>
       </c>
       <c r="B317" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C317" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="C317" s="5" t="s">
-        <v>234</v>
-      </c>
       <c r="D317" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E317" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="318" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6474,7 +6561,7 @@
         <v>4</v>
       </c>
       <c r="B318" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C318" s="5" t="s">
         <v>140</v>
@@ -6491,16 +6578,16 @@
         <v>5</v>
       </c>
       <c r="B319" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C319" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D319" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E319" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="D319" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E319" s="6" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="321" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6508,16 +6595,16 @@
         <v>1</v>
       </c>
       <c r="B321" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C321" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D321" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E321" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="322" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6525,16 +6612,16 @@
         <v>2</v>
       </c>
       <c r="B322" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C322" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C322" s="5" t="s">
-        <v>239</v>
-      </c>
       <c r="D322" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E322" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="323" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6542,16 +6629,16 @@
         <v>3</v>
       </c>
       <c r="B323" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C323" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D323" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E323" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="324" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6559,16 +6646,16 @@
         <v>4</v>
       </c>
       <c r="B324" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C324" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D324" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E324" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="325" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6576,16 +6663,16 @@
         <v>5</v>
       </c>
       <c r="B325" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C325" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D325" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E325" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="326" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6593,16 +6680,16 @@
         <v>6</v>
       </c>
       <c r="B326" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C326" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D326" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E326" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="328" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6610,7 +6697,7 @@
         <v>1</v>
       </c>
       <c r="B328" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C328" s="5" t="s">
         <v>139</v>
@@ -6627,16 +6714,16 @@
         <v>2</v>
       </c>
       <c r="B329" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C329" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D329" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E329" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="330" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6644,16 +6731,16 @@
         <v>3</v>
       </c>
       <c r="B330" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C330" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D330" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E330" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="331" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6661,16 +6748,16 @@
         <v>4</v>
       </c>
       <c r="B331" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C331" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D331" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E331" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="332" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6678,16 +6765,16 @@
         <v>5</v>
       </c>
       <c r="B332" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C332" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D332" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E332" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="333" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6695,7 +6782,7 @@
         <v>6</v>
       </c>
       <c r="B333" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C333" s="5" t="s">
         <v>140</v>
@@ -6712,16 +6799,16 @@
         <v>7</v>
       </c>
       <c r="B334" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C334" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="C334" s="5" t="s">
-        <v>246</v>
-      </c>
       <c r="D334" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E334" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="336" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6729,7 +6816,7 @@
         <v>1</v>
       </c>
       <c r="B336" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C336" s="5" t="s">
         <v>139</v>
@@ -6746,16 +6833,16 @@
         <v>2</v>
       </c>
       <c r="B337" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C337" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D337" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E337" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="338" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6763,16 +6850,16 @@
         <v>3</v>
       </c>
       <c r="B338" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C338" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D338" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E338" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="339" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6780,16 +6867,16 @@
         <v>4</v>
       </c>
       <c r="B339" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C339" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D339" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E339" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="340" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6797,16 +6884,16 @@
         <v>5</v>
       </c>
       <c r="B340" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C340" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="C340" s="5" t="s">
-        <v>244</v>
-      </c>
       <c r="D340" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E340" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="341" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6814,7 +6901,7 @@
         <v>6</v>
       </c>
       <c r="B341" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C341" s="5" t="s">
         <v>140</v>
@@ -6831,16 +6918,16 @@
         <v>7</v>
       </c>
       <c r="B342" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C342" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D342" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E342" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="344" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6848,16 +6935,16 @@
         <v>1</v>
       </c>
       <c r="B344" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C344" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="C344" s="5" t="s">
-        <v>231</v>
-      </c>
       <c r="D344" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E344" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="345" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6865,16 +6952,16 @@
         <v>2</v>
       </c>
       <c r="B345" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C345" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D345" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E345" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="346" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6882,16 +6969,16 @@
         <v>3</v>
       </c>
       <c r="B346" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C346" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D346" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E346" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="348" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6899,16 +6986,16 @@
         <v>1</v>
       </c>
       <c r="B348" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C348" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D348" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E348" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="349" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6916,16 +7003,16 @@
         <v>2</v>
       </c>
       <c r="B349" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C349" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D349" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E349" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="C349" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="D349" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E349" s="6" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="350" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6933,16 +7020,16 @@
         <v>3</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C350" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D350" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E350" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="351" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6950,16 +7037,16 @@
         <v>4</v>
       </c>
       <c r="B351" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C351" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D351" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E351" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="352" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6967,7 +7054,7 @@
         <v>5</v>
       </c>
       <c r="B352" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C352" s="5" t="s">
         <v>12</v>
@@ -6984,16 +7071,16 @@
         <v>6</v>
       </c>
       <c r="B353" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C353" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D353" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E353" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="354" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7001,16 +7088,16 @@
         <v>7</v>
       </c>
       <c r="B354" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C354" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D354" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E354" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="355" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7018,7 +7105,7 @@
         <v>8</v>
       </c>
       <c r="B355" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C355" s="5" t="s">
         <v>27</v>
@@ -7035,7 +7122,7 @@
         <v>9</v>
       </c>
       <c r="B356" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C356" s="5" t="s">
         <v>29</v>
@@ -7052,7 +7139,7 @@
         <v>10</v>
       </c>
       <c r="B357" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C357" s="5" t="s">
         <v>31</v>
@@ -7069,7 +7156,7 @@
         <v>11</v>
       </c>
       <c r="B358" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C358" s="5" t="s">
         <v>25</v>
@@ -7378,7 +7465,7 @@
         <v>99</v>
       </c>
       <c r="C378" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D378" s="6" t="s">
         <v>15</v>
@@ -7545,7 +7632,7 @@
         <v>1</v>
       </c>
       <c r="B390" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C390" s="5" t="s">
         <v>12</v>
@@ -7562,10 +7649,10 @@
         <v>2</v>
       </c>
       <c r="B391" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C391" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D391" s="6" t="s">
         <v>15</v>
@@ -7579,7 +7666,7 @@
         <v>3</v>
       </c>
       <c r="B392" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C392" s="5" t="s">
         <v>25</v>
@@ -7596,7 +7683,7 @@
         <v>4</v>
       </c>
       <c r="B393" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C393" s="5" t="s">
         <v>101</v>
@@ -7613,7 +7700,7 @@
         <v>5</v>
       </c>
       <c r="B394" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C394" s="5" t="s">
         <v>102</v>
@@ -7630,7 +7717,7 @@
         <v>6</v>
       </c>
       <c r="B395" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C395" s="5" t="s">
         <v>12</v>
@@ -7647,10 +7734,10 @@
         <v>7</v>
       </c>
       <c r="B396" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C396" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D396" s="6" t="s">
         <v>15</v>
@@ -7664,7 +7751,7 @@
         <v>8</v>
       </c>
       <c r="B397" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C397" s="5" t="s">
         <v>25</v>
@@ -7681,7 +7768,7 @@
         <v>1</v>
       </c>
       <c r="B399" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C399" s="6" t="s">
         <v>12</v>
@@ -7698,16 +7785,16 @@
         <v>2</v>
       </c>
       <c r="B400" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C400" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="D400" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E400" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="C400" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="D400" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E400" s="6" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
@@ -7715,7 +7802,7 @@
         <v>3</v>
       </c>
       <c r="B401" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C401" s="6" t="s">
         <v>25</v>
@@ -7732,7 +7819,7 @@
         <v>1</v>
       </c>
       <c r="B403" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C403" s="6" t="s">
         <v>12</v>
@@ -7749,16 +7836,16 @@
         <v>2</v>
       </c>
       <c r="B404" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C404" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D404" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E404" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="C404" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="D404" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E404" s="6" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
@@ -7766,7 +7853,7 @@
         <v>3</v>
       </c>
       <c r="B405" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C405" s="6" t="s">
         <v>25</v>
@@ -7783,7 +7870,7 @@
         <v>1</v>
       </c>
       <c r="B407" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C407" s="6" t="s">
         <v>12</v>
@@ -7800,16 +7887,16 @@
         <v>2</v>
       </c>
       <c r="B408" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C408" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D408" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E408" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
@@ -7817,7 +7904,7 @@
         <v>3</v>
       </c>
       <c r="B409" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C409" s="6" t="s">
         <v>25</v>
@@ -7830,348 +7917,348 @@
       </c>
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A411" s="13">
+      <c r="A411" s="11">
         <v>1</v>
       </c>
-      <c r="B411" s="14" t="s">
+      <c r="B411" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C411" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D411" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E411" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A412" s="11">
+        <v>2</v>
+      </c>
+      <c r="B412" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C412" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D412" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E412" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A413" s="11">
+        <v>3</v>
+      </c>
+      <c r="B413" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C413" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D413" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E413" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A414" s="11">
+        <v>4</v>
+      </c>
+      <c r="B414" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C414" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D414" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E414" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A415" s="11">
+        <v>5</v>
+      </c>
+      <c r="B415" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C415" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D415" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E415" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A416" s="11">
+        <v>6</v>
+      </c>
+      <c r="B416" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C416" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="C411" s="15" t="s">
+      <c r="D416" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E416" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A417" s="11">
+        <v>7</v>
+      </c>
+      <c r="B417" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C417" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D417" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E417" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A418" s="11"/>
+      <c r="B418" s="11"/>
+      <c r="C418" s="11"/>
+      <c r="D418" s="11"/>
+      <c r="E418" s="11"/>
+    </row>
+    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A419" s="11">
+        <v>1</v>
+      </c>
+      <c r="B419" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C419" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D411" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E411" s="16" t="s">
+      <c r="D419" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E419" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A412" s="13">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A420" s="11">
         <v>2</v>
       </c>
-      <c r="B412" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="C412" s="15" t="s">
+      <c r="B420" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C420" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D412" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E412" s="16" t="s">
+      <c r="D420" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E420" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A413" s="13">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A421" s="11">
         <v>3</v>
       </c>
-      <c r="B413" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="C413" s="15" t="s">
+      <c r="B421" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C421" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D413" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E413" s="16" t="s">
+      <c r="D421" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E421" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A414" s="13">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A422" s="11">
         <v>4</v>
       </c>
-      <c r="B414" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="C414" s="15" t="s">
+      <c r="B422" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C422" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D414" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E414" s="16" t="s">
+      <c r="D422" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E422" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A415" s="13">
-        <v>5</v>
-      </c>
-      <c r="B415" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="C415" s="15" t="s">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A423" s="11">
+        <v>5</v>
+      </c>
+      <c r="B423" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C423" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D415" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E415" s="16" t="s">
+      <c r="D423" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E423" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A416" s="13">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A424" s="11">
         <v>6</v>
       </c>
-      <c r="B416" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="C416" s="15" t="s">
+      <c r="B424" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="D416" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E416" s="16" t="s">
+      <c r="C424" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D424" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E424" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A417" s="13">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A425" s="11">
         <v>7</v>
       </c>
-      <c r="B417" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="C417" s="15" t="s">
+      <c r="B425" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C425" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D417" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E417" s="16" t="s">
+      <c r="D425" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E425" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A418" s="13"/>
-      <c r="B418" s="17"/>
-      <c r="C418" s="17"/>
-      <c r="D418" s="17"/>
-      <c r="E418" s="17"/>
-    </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A419" s="13">
-        <v>1</v>
-      </c>
-      <c r="B419" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C419" s="15" t="s">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A426" s="11">
+        <v>8</v>
+      </c>
+      <c r="B426" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C426" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D426" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E426" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A427" s="11">
+        <v>9</v>
+      </c>
+      <c r="B427" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C427" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="D427" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E427" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A428" s="11">
+        <v>10</v>
+      </c>
+      <c r="B428" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C428" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D419" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E419" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A420" s="13">
-        <v>2</v>
-      </c>
-      <c r="B420" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C420" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D420" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E420" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A421" s="13">
-        <v>3</v>
-      </c>
-      <c r="B421" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C421" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D421" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E421" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A422" s="13">
-        <v>4</v>
-      </c>
-      <c r="B422" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C422" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D422" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E422" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A423" s="13">
-        <v>5</v>
-      </c>
-      <c r="B423" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C423" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D423" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E423" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A424" s="13">
-        <v>6</v>
-      </c>
-      <c r="B424" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C424" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="D424" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E424" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A425" s="13">
-        <v>7</v>
-      </c>
-      <c r="B425" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C425" s="15" t="s">
+      <c r="D428" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E428" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A429" s="11">
+        <v>11</v>
+      </c>
+      <c r="B429" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C429" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="D429" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E429" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A430" s="11">
+        <v>12</v>
+      </c>
+      <c r="B430" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C430" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D425" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E425" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A426" s="13">
-        <v>8</v>
-      </c>
-      <c r="B426" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C426" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D426" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E426" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A427" s="13">
-        <v>9</v>
-      </c>
-      <c r="B427" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C427" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="D427" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E427" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A428" s="13">
-        <v>10</v>
-      </c>
-      <c r="B428" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C428" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D428" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E428" s="16" t="s">
+      <c r="D430" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E430" s="14" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A429" s="13">
-        <v>11</v>
-      </c>
-      <c r="B429" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C429" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="D429" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E429" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A430" s="13">
-        <v>12</v>
-      </c>
-      <c r="B430" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="C430" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D430" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E430" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A431" s="18"/>
-      <c r="B431" s="14"/>
-      <c r="C431" s="16"/>
-      <c r="D431" s="16"/>
-      <c r="E431" s="16"/>
+      <c r="A431" s="11"/>
+      <c r="B431" s="12"/>
+      <c r="C431" s="14"/>
+      <c r="D431" s="14"/>
+      <c r="E431" s="14"/>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A432" s="3">
         <v>1</v>
       </c>
       <c r="B432" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C432" s="6" t="s">
         <v>12</v>
@@ -8188,10 +8275,10 @@
         <v>2</v>
       </c>
       <c r="B433" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C433" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="C433" s="6" t="s">
-        <v>272</v>
       </c>
       <c r="D433" s="6" t="s">
         <v>15</v>
@@ -8205,7 +8292,7 @@
         <v>3</v>
       </c>
       <c r="B434" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C434" s="6" t="s">
         <v>25</v>
@@ -8217,126 +8304,659 @@
         <v>26</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B435" s="8"/>
-    </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A436">
+      <c r="A436" s="3">
         <v>1</v>
       </c>
-      <c r="B436" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="C436" s="6" t="s">
-        <v>12</v>
+      <c r="B436" s="8"/>
+      <c r="C436" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="D436" s="6" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E436" s="6" t="s">
-        <v>13</v>
+        <v>139</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A437">
+      <c r="A437" s="3">
         <v>2</v>
       </c>
       <c r="B437" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="C437" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
+      </c>
+      <c r="C437" s="5" t="s">
+        <v>214</v>
       </c>
       <c r="D437" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E437" s="6" t="s">
-        <v>128</v>
+        <v>214</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A438">
-        <v>1</v>
+      <c r="A438" s="3">
+        <v>3</v>
       </c>
       <c r="B438" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="C438" s="6" t="s">
-        <v>12</v>
+      <c r="C438" s="5" t="s">
+        <v>238</v>
       </c>
       <c r="D438" s="6" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E438" s="6" t="s">
-        <v>13</v>
+        <v>238</v>
       </c>
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A439">
-        <v>2</v>
+      <c r="A439" s="3">
+        <v>4</v>
       </c>
       <c r="B439" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="C439" s="6" t="s">
-        <v>291</v>
+      <c r="C439" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="D439" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E439" s="6" t="s">
-        <v>128</v>
+        <v>239</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A440">
-        <v>3</v>
+      <c r="A440" s="3">
+        <v>5</v>
       </c>
       <c r="B440" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="C440" s="6" t="s">
+      <c r="C440" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D440" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E440" s="6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A441" s="3">
+        <v>6</v>
+      </c>
+      <c r="B441" s="8"/>
+      <c r="C441" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D441" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E441" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A442" s="3">
+        <v>7</v>
+      </c>
+      <c r="B442" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C442" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D442" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E442" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A444" s="3">
+        <v>1</v>
+      </c>
+      <c r="B444" s="8"/>
+      <c r="C444" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D444" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E444" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A445" s="3">
+        <v>2</v>
+      </c>
+      <c r="B445" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C445" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D445" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E445" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A446" s="3">
+        <v>3</v>
+      </c>
+      <c r="B446" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C446" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D446" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E446" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A447" s="3">
+        <v>4</v>
+      </c>
+      <c r="B447" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C447" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D447" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E447" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A448" s="3">
+        <v>5</v>
+      </c>
+      <c r="B448" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C448" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D448" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E448" s="6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A449" s="3">
+        <v>6</v>
+      </c>
+      <c r="B449" s="8"/>
+      <c r="C449" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D449" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E449" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A450" s="3">
+        <v>7</v>
+      </c>
+      <c r="B450" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C450" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D450" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E450" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A451" s="3">
+        <v>8</v>
+      </c>
+      <c r="B451" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C451" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D451" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E451" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A453" s="3">
+        <v>1</v>
+      </c>
+      <c r="B453" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C453" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D453" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E453" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A454" s="3">
+        <v>2</v>
+      </c>
+      <c r="B454" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C454" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D454" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E454" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A455" s="3">
+        <v>3</v>
+      </c>
+      <c r="B455" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C455" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D455" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E455" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A456" s="3">
+        <v>4</v>
+      </c>
+      <c r="B456" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C456" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D456" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E456" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A457" s="3">
+        <v>5</v>
+      </c>
+      <c r="B457" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C457" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="D440" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E440" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A441">
+      <c r="D457" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E457" s="6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A459" s="3">
         <v>1</v>
       </c>
-      <c r="B441" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="C441" s="6" t="s">
+      <c r="B459" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C459" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D441" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E441" s="6" t="s">
+      <c r="D459" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E459" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A442">
+    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A460" s="3">
         <v>2</v>
       </c>
-      <c r="B442" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="C442" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="D442" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E442" s="6" t="s">
-        <v>128</v>
+      <c r="B460" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C460" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D460" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E460" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A461" s="3">
+        <v>3</v>
+      </c>
+      <c r="B461" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C461" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D461" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E461" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A462" s="3">
+        <v>4</v>
+      </c>
+      <c r="B462" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C462" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D462" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E462" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A463" s="3">
+        <v>5</v>
+      </c>
+      <c r="B463" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C463" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D463" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E463" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A464" s="3">
+        <v>6</v>
+      </c>
+      <c r="B464" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C464" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D464" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E464" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A465" s="3">
+        <v>7</v>
+      </c>
+      <c r="B465" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C465" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D465" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E465" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A466" s="3">
+        <v>8</v>
+      </c>
+      <c r="B466" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C466" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D466" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E466" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A467" s="3">
+        <v>9</v>
+      </c>
+      <c r="B467" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C467" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D467" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E467" s="6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A468" s="3">
+        <v>10</v>
+      </c>
+      <c r="B468" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C468" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D468" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E468" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A470" s="3">
+        <v>1</v>
+      </c>
+      <c r="B470" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C470" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D470" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E470" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="471" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A471" s="3">
+        <v>2</v>
+      </c>
+      <c r="B471" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C471" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D471" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E471" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A472" s="3">
+        <v>3</v>
+      </c>
+      <c r="B472" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C472" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D472" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E472" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A473" s="3">
+        <v>4</v>
+      </c>
+      <c r="B473" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C473" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D473" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E473" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A474" s="3">
+        <v>5</v>
+      </c>
+      <c r="B474" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C474" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D474" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E474" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="475" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A475" s="3">
+        <v>6</v>
+      </c>
+      <c r="B475" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C475" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="D475" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E475" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="477" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A477" s="3">
+        <v>1</v>
+      </c>
+      <c r="B477" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C477" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D477" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E477" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A478" s="3">
+        <v>2</v>
+      </c>
+      <c r="B478" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C478" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D478" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E478" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A479" s="3">
+        <v>3</v>
+      </c>
+      <c r="B479" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C479" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="D479" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E479" s="5" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -8350,7 +8970,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -8983,7 +9603,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>